<commit_message>
patch for la Rochelle
</commit_message>
<xml_diff>
--- a/Data Sheets/Sandbox.xlsx
+++ b/Data Sheets/Sandbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\themi\AppData\LocalLow\Deep Water Studio\UBOAT\Mods\wip-expanded-convoys-and-shipping-lanes\Data Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33A8028-5E9A-42D5-B9C1-39EA92D31029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC743540-1BBF-4DC5-B53C-84278A42F42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="30570" windowHeight="19410" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1425" windowWidth="30570" windowHeight="19410" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="436">
   <si>
     <t>Group Name</t>
   </si>
@@ -1338,6 +1338,9 @@
   </si>
   <si>
     <t>Submarine (0, 1, 0.8, 0.5, 0.25, 0.1)</t>
+  </si>
+  <si>
+    <t>Corvette (1, 0.2); Fast Attack Craft (0.25, 1, 0.75, 0.5)</t>
   </si>
 </sst>
 </file>
@@ -16381,13 +16384,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
+      <selection pane="bottomRight" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16448,7 +16452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="7" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>232</v>
       </c>
@@ -16487,7 +16491,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="7" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>234</v>
       </c>
@@ -16528,7 +16532,7 @@
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
     </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="9" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>91</v>
       </c>
@@ -16569,7 +16573,7 @@
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>381</v>
       </c>
@@ -16608,7 +16612,7 @@
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>361</v>
       </c>
@@ -16647,7 +16651,7 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>326</v>
       </c>
@@ -16688,7 +16692,7 @@
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>215</v>
       </c>
@@ -16729,7 +16733,7 @@
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
     </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="9" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>365</v>
       </c>
@@ -16768,7 +16772,7 @@
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
     </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="9" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>34</v>
       </c>
@@ -16809,7 +16813,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
     </row>
-    <row r="11" spans="1:15" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="9" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>172</v>
       </c>
@@ -16850,7 +16854,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>338</v>
       </c>
@@ -16891,7 +16895,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>332</v>
       </c>
@@ -16932,7 +16936,7 @@
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
     </row>
-    <row r="14" spans="1:15" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="23" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>288</v>
       </c>
@@ -16973,7 +16977,7 @@
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
     </row>
-    <row r="15" spans="1:15" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="23" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>300</v>
       </c>
@@ -17014,7 +17018,7 @@
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>317</v>
       </c>
@@ -17055,7 +17059,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
     </row>
-    <row r="17" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>394</v>
       </c>
@@ -17096,7 +17100,7 @@
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
     </row>
-    <row r="18" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>360</v>
       </c>
@@ -17135,7 +17139,7 @@
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>379</v>
       </c>
@@ -17174,7 +17178,7 @@
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>340</v>
       </c>
@@ -17215,7 +17219,7 @@
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>323</v>
       </c>
@@ -17270,7 +17274,7 @@
         <v>102</v>
       </c>
       <c r="E22" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="23">
         <v>1000</v>
@@ -17311,7 +17315,7 @@
         <v>102</v>
       </c>
       <c r="E23" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="23">
         <v>1000</v>
@@ -17331,10 +17335,10 @@
       <c r="K23" s="23"/>
       <c r="L23" s="19"/>
       <c r="M23" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="25" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>87</v>
       </c>
@@ -17372,7 +17376,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="7" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>122</v>
       </c>
@@ -17413,7 +17417,7 @@
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>223</v>
       </c>
@@ -17454,7 +17458,7 @@
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>157</v>
       </c>
@@ -17495,7 +17499,7 @@
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>204</v>
       </c>
@@ -17536,7 +17540,7 @@
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>127</v>
       </c>
@@ -17577,7 +17581,7 @@
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>170</v>
       </c>
@@ -17618,7 +17622,7 @@
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>380</v>
       </c>
@@ -17657,7 +17661,7 @@
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>254</v>
       </c>
@@ -17698,7 +17702,7 @@
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>321</v>
       </c>
@@ -17739,7 +17743,7 @@
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>40</v>
       </c>
@@ -17780,7 +17784,7 @@
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>329</v>
       </c>
@@ -17821,7 +17825,7 @@
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>233</v>
       </c>
@@ -17862,7 +17866,7 @@
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>137</v>
       </c>
@@ -17903,7 +17907,7 @@
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="7" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>133</v>
       </c>
@@ -17944,7 +17948,7 @@
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="7" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>370</v>
       </c>
@@ -17983,7 +17987,7 @@
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>368</v>
       </c>
@@ -18022,7 +18026,7 @@
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>335</v>
       </c>
@@ -18063,7 +18067,7 @@
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>145</v>
       </c>
@@ -18104,7 +18108,7 @@
       <c r="N42" s="15"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>359</v>
       </c>
@@ -18143,7 +18147,7 @@
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="7" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>63</v>
       </c>
@@ -18184,7 +18188,7 @@
       <c r="N44" s="15"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>222</v>
       </c>
@@ -18223,7 +18227,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>224</v>
       </c>
@@ -18261,7 +18265,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>219</v>
       </c>
@@ -18302,7 +18306,7 @@
       <c r="N47" s="15"/>
       <c r="O47" s="15"/>
     </row>
-    <row r="48" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>228</v>
       </c>
@@ -18340,7 +18344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>348</v>
       </c>
@@ -18378,7 +18382,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>60</v>
       </c>
@@ -18419,7 +18423,7 @@
       <c r="N50" s="15"/>
       <c r="O50" s="15"/>
     </row>
-    <row r="51" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>342</v>
       </c>
@@ -18458,7 +18462,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>307</v>
       </c>
@@ -18496,7 +18500,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="15" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>297</v>
       </c>
@@ -18534,7 +18538,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>315</v>
       </c>
@@ -18573,7 +18577,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>310</v>
       </c>
@@ -18611,7 +18615,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>294</v>
       </c>
@@ -18649,7 +18653,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>313</v>
       </c>
@@ -18687,7 +18691,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
         <v>413</v>
       </c>
@@ -18726,7 +18730,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>417</v>
       </c>
@@ -18765,7 +18769,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>419</v>
       </c>
@@ -18804,7 +18808,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>202</v>
       </c>
@@ -18842,7 +18846,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>218</v>
       </c>
@@ -18918,7 +18922,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>212</v>
       </c>
@@ -18956,7 +18960,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>302</v>
       </c>
@@ -18995,7 +18999,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>140</v>
       </c>
@@ -19033,7 +19037,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>82</v>
       </c>
@@ -19146,7 +19150,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>71</v>
       </c>
@@ -19185,7 +19189,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>118</v>
       </c>
@@ -19224,7 +19228,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="15" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>80</v>
       </c>
@@ -19262,7 +19266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
         <v>206</v>
       </c>
@@ -19300,7 +19304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>211</v>
       </c>
@@ -19338,7 +19342,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>347</v>
       </c>
@@ -19377,7 +19381,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="15" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>346</v>
       </c>
@@ -19416,7 +19420,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="23" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
         <v>159</v>
       </c>
@@ -19455,7 +19459,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
         <v>55</v>
       </c>
@@ -19494,7 +19498,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
         <v>116</v>
       </c>
@@ -19533,7 +19537,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="25" t="s">
         <v>154</v>
       </c>
@@ -19572,7 +19576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="26" t="s">
         <v>124</v>
       </c>
@@ -19611,7 +19615,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
         <v>291</v>
       </c>
@@ -19649,7 +19653,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="23" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
         <v>305</v>
       </c>
@@ -19688,7 +19692,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="23" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" s="23" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
         <v>319</v>
       </c>
@@ -19727,7 +19731,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" s="23" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="21" t="s">
         <v>95</v>
       </c>
@@ -19766,7 +19770,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" s="23" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
         <v>236</v>
       </c>
@@ -19804,7 +19808,7 @@
       <c r="N86" s="25"/>
       <c r="O86" s="25"/>
     </row>
-    <row r="87" spans="1:15" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" s="25" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
         <v>34</v>
       </c>
@@ -19839,7 +19843,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" s="25" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
         <v>432</v>
       </c>
@@ -19874,7 +19878,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" s="25" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
         <v>105</v>
       </c>
@@ -19912,6 +19916,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M89" xr:uid="{3E33B360-02B2-431A-9C72-00D27FB0981C}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Coastal Defense Patrol"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M89">
       <sortCondition ref="I1:I89"/>
     </sortState>

</xml_diff>